<commit_message>
updating to latest repo
</commit_message>
<xml_diff>
--- a/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
+++ b/src/main/resources/CompilerDictionary/KeywordDictionary/KeywordDictionaryForWebTesting.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" calcMode="manual"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Sno</t>
   </si>
@@ -137,6 +137,33 @@
   </si>
   <si>
     <t>Accepts no parameters and waits for page to render itself. It does that by observing network state. Step never triggers test failure and waits for maximum period of 30 seconds</t>
+  </si>
+  <si>
+    <t>textBoxShouldHaveValue</t>
+  </si>
+  <si>
+    <t>Accepts two parameters @locator and @testData. It gets the text from textBox and validates against the @testData provided. If the validation fails testing should still continue</t>
+  </si>
+  <si>
+    <t>elementShouldNotBePresent</t>
+  </si>
+  <si>
+    <t>Accepts no parameters and verifies element is not available in DOM. Returns true if element is not available in DOM</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>isButtonEnabled</t>
+  </si>
+  <si>
+    <t>isButtonDisabled</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Checks if the Button is enabled. Returns true if the button is enabled</t>
+  </si>
+  <si>
+    <t>Accepts one parameter @locator. Checks if the Button is disabled Returns true if the button is disabled</t>
   </si>
 </sst>
 </file>
@@ -180,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -189,6 +216,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -733,13 +762,69 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>